<commit_message>
Doan day danh sach loi 13/12/2019
</commit_message>
<xml_diff>
--- a/5.Reference/191111_TrienKhai_ThanhThuy/191202_Loi_Sua_ThanhThuy.xlsx
+++ b/5.Reference/191111_TrienKhai_ThanhThuy/191202_Loi_Sua_ThanhThuy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C61078-DB04-4590-907E-101A9400C990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236C68C3-7A1D-4CC1-A4CB-97D02B9BFF38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="65">
   <si>
     <t>TT</t>
   </si>
@@ -233,12 +233,38 @@
     <t>Tính toán số lượng đáp ứng theo các yêu cầu xuất kho</t>
   </si>
   <si>
+    <t>Phiếu xuất kho</t>
+  </si>
+  <si>
+    <t>Xuất phiếu xuất kho</t>
+  </si>
+  <si>
+    <t>Chân ký đầu tiên đang bị đẩy lên 1 dòng so với chân ký khác</t>
+  </si>
+  <si>
+    <t>Các chân ký thành hàng</t>
+  </si>
+  <si>
     <t>-Trường Ghi chú đang lấy thông tin từ db.
-- Các border trong bảng hàng hóa có chỗ đậm chỗ nhạt.</t>
+-Các border trong bảng hàng hóa có chỗ đậm chỗ nhạt.
+-Độ rộng các cột không hợp lý với dữ liệu thực tế</t>
   </si>
   <si>
     <t>-Trường Ghi chú luôn để trống.
-- Các border trong bảng hàng hóa để cùng kích thước.</t>
+-Các border trong bảng hàng hóa để cùng kích thước.
+-Căn độ rộng các cột theo như ảnh chụp đã gửi trong skype</t>
+  </si>
+  <si>
+    <t>Thực hiện lỗi số 2 trước khi thực hiện lỗi này</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Doanh thu bán hàng theo ngày</t>
+  </si>
+  <si>
+    <t>Định hướng sản phẩm ko hỗ trợ nghiệp vụ này =&gt; không cần tổng hợp dữ liệu đẩy vào bảng nghiệp vụ nữa đỡ tốn dung lượng</t>
   </si>
 </sst>
 </file>
@@ -1151,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E2F3C4-2138-42F6-A480-FF60B111EBE3}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1237,7 +1263,7 @@
       </c>
       <c r="K2" s="29"/>
     </row>
-    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1251,10 +1277,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>15</v>
@@ -1298,7 +1324,9 @@
       <c r="J4" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="27"/>
+      <c r="K4" s="27" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
@@ -1332,6 +1360,70 @@
       <c r="K5" s="31" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="15">
+        <v>43720</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="30"/>
+    </row>
+    <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="15">
+        <v>43720</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="30"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -1339,7 +1431,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{0BCB52E2-9031-4C94-9AFD-7ED6FE65F201}">
       <formula1>"New, Resolve, Confirm, Close, Cancel, Accept"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1048576" xr:uid="{75FEF98B-C920-4027-A76B-EAC5F541C030}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6 D8:D1048576" xr:uid="{75FEF98B-C920-4027-A76B-EAC5F541C030}">
       <formula1>"Lỗi, Đề xuất"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>